<commit_message>
added Logic in Excel
</commit_message>
<xml_diff>
--- a/excel/src/logic_in_excel.xlsx
+++ b/excel/src/logic_in_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scottish-my.sharepoint.com/personal/brendan_clarke2_nes_scot_nhs_uk/Documents/projects/KIND resources/excel_logic/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brendancl\not_od\KIND-training\excel\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{88A7EC97-91C5-4DC2-B722-C6FDC94937EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5CA9A17-7FA6-48FE-9C38-FE3EA2169620}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002CE95-F997-4C55-8290-01AC434BA2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="18240" activeTab="6" xr2:uid="{462B433E-3A6E-446E-BD28-09DA4E5466BF}"/>
+    <workbookView xWindow="29850" yWindow="-120" windowWidth="27870" windowHeight="16440" firstSheet="3" activeTab="6" xr2:uid="{462B433E-3A6E-446E-BD28-09DA4E5466BF}"/>
   </bookViews>
   <sheets>
     <sheet name="NOT" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>P</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>grows</t>
+  </si>
+  <si>
+    <t>No CRD</t>
+  </si>
+  <si>
+    <t>Nothing</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1673,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,8 +1699,8 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3">
         <v>27</v>
@@ -1711,23 +1717,23 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4" t="str" cm="1">
         <f t="array" ref="E4">_xlfn.IFS(B4 = TRUE,"High",C4 = "CRD","High", D4 &gt; 20,"High", TRUE,"Low")</f>
-        <v>Low</v>
+        <v>High</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>99</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -1741,8 +1747,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>99</v>
       </c>
       <c r="D6">
         <v>26</v>
@@ -1756,23 +1762,23 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
       <c r="D7">
         <v>15</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xlfn.IFS(B7 = TRUE,"High",C7 = "CRD","High", D7 &gt; 20,"High", TRUE,"Low")</f>
-        <v>Low</v>
+        <v>High</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>99</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -1786,8 +1792,8 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>99</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -1801,8 +1807,8 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
+      <c r="C10" t="s">
+        <v>99</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1816,23 +1822,23 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>16</v>
       </c>
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.IFS(B11 = TRUE,"High",C11 = "CRD","High", D11 &gt; 20,"High", TRUE,"Low")</f>
-        <v>Low</v>
+        <v>High</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>100</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -2024,7 +2030,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FAB9AB-A287-4E63-937E-C690CE660694}">
   <dimension ref="B2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>

</xml_diff>